<commit_message>
IZMENENIYA DLYA VETKI 2
</commit_message>
<xml_diff>
--- a/SecondFile.xlsx
+++ b/SecondFile.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ba</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>ag</t>
+  </si>
+  <si>
+    <t>VETKA 22222222</t>
   </si>
 </sst>
 </file>
@@ -363,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T16"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +418,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>